<commit_message>
[update] test case Chia Kênh
</commit_message>
<xml_diff>
--- a/Data/TestCase_ChiaKenh.xlsx
+++ b/Data/TestCase_ChiaKenh.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAP60536_Local\Downloads\Exercise-main\Exercise-main\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CPU60246-Fresher\IdeaProjects\Exercise\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="39">
   <si>
     <t xml:space="preserve">Test case </t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>closeWeb</t>
-  </si>
-  <si>
-    <t>Client2</t>
   </si>
 </sst>
 </file>
@@ -726,10 +723,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD18"/>
+      <selection activeCell="A16" sqref="A16:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,7 +890,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -904,9 +901,11 @@
         <v>15</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="16"/>
+        <v>19</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -916,17 +915,57 @@
         <v>15</v>
       </c>
       <c r="C18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>8</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>9</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>10</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="16"/>
-    </row>
-    <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="D21" s="16"/>
+    </row>
+    <row r="22" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="14"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -935,10 +974,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD18"/>
+      <selection activeCell="A16" sqref="A16:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,7 +1141,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1113,9 +1152,11 @@
         <v>15</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="16"/>
+        <v>19</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -1125,17 +1166,57 @@
         <v>15</v>
       </c>
       <c r="C18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>8</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>9</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>10</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="16"/>
-    </row>
-    <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="D21" s="16"/>
+    </row>
+    <row r="22" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="14"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1144,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD18"/>
+      <selection activeCell="A16" sqref="A16:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1311,7 +1392,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1322,9 +1403,11 @@
         <v>15</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="16"/>
+        <v>19</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -1334,17 +1417,57 @@
         <v>15</v>
       </c>
       <c r="C18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>8</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>9</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>10</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="16"/>
-    </row>
-    <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="D21" s="16"/>
+    </row>
+    <row r="22" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="14"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1353,10 +1476,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,7 +1643,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1531,9 +1654,11 @@
         <v>15</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="16"/>
+        <v>19</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -1543,17 +1668,57 @@
         <v>15</v>
       </c>
       <c r="C18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>8</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>9</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>10</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="16"/>
-    </row>
-    <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="D21" s="16"/>
+    </row>
+    <row r="22" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="14"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1861,10 +2026,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2039,9 +2204,11 @@
         <v>15</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="16"/>
+        <v>19</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -2051,21 +2218,25 @@
         <v>15</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="16"/>
+        <v>19</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>8</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="16"/>
+        <v>19</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="20" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
@@ -2075,17 +2246,29 @@
         <v>15</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D20" s="16"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>10</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="16"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="14"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2094,10 +2277,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD18"/>
+      <selection activeCell="A17" sqref="A17:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2272,9 +2455,11 @@
         <v>15</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="16"/>
+        <v>19</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -2284,17 +2469,57 @@
         <v>15</v>
       </c>
       <c r="C18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>8</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>9</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>10</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="16"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="D21" s="16"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="14"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2303,10 +2528,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD18"/>
+      <selection activeCell="A17" sqref="A17:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2481,9 +2706,11 @@
         <v>15</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="16"/>
+        <v>19</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -2493,17 +2720,57 @@
         <v>15</v>
       </c>
       <c r="C18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>8</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>9</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>10</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="16"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="D21" s="16"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="14"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2512,10 +2779,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD18"/>
+      <selection activeCell="A16" sqref="A16:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2690,9 +2957,11 @@
         <v>15</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="16"/>
+        <v>19</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -2702,17 +2971,57 @@
         <v>15</v>
       </c>
       <c r="C18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>8</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>9</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>10</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="16"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="D21" s="16"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="14"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2721,10 +3030,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD18"/>
+      <selection activeCell="A16" sqref="A16:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2888,7 +3197,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2899,9 +3208,11 @@
         <v>15</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="16"/>
+        <v>19</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -2911,17 +3222,57 @@
         <v>15</v>
       </c>
       <c r="C18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>8</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>9</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>10</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="16"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="D21" s="16"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="14"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2930,10 +3281,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD18"/>
+      <selection activeCell="A16" sqref="A16:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3097,7 +3448,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3108,9 +3459,11 @@
         <v>15</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="16"/>
+        <v>19</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -3120,17 +3473,57 @@
         <v>15</v>
       </c>
       <c r="C18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>8</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>9</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>10</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="16"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="D21" s="16"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="14"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3139,10 +3532,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD18"/>
+      <selection activeCell="A12" sqref="A12:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3306,7 +3699,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3317,9 +3710,11 @@
         <v>15</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="16"/>
+        <v>19</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -3329,17 +3724,57 @@
         <v>15</v>
       </c>
       <c r="C18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>8</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>9</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>10</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="16"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="D21" s="16"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="14"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3348,10 +3783,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD18"/>
+      <selection activeCell="A16" sqref="A16:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3515,7 +3950,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3526,9 +3961,11 @@
         <v>15</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="16"/>
+        <v>19</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -3538,17 +3975,57 @@
         <v>15</v>
       </c>
       <c r="C18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>8</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>9</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>10</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="16"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="D21" s="16"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="14"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>